<commit_message>
Changed Boroughs to Name in 2014 data
</commit_message>
<xml_diff>
--- a/2014 data.xlsx
+++ b/2014 data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/alyssa/code/alyssageorgee/group23/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{87BA7B49-63B8-C241-B8B6-0F05794D51BA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0F8682FC-0141-0243-9A8C-6ADFF45F1546}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="3960" yWindow="500" windowWidth="24460" windowHeight="16200" xr2:uid="{37C820EF-1D58-D945-81CF-68D7AB62C7C7}"/>
   </bookViews>
@@ -39,9 +39,6 @@
     <t>Suicide Rates</t>
   </si>
   <si>
-    <t>Broughs</t>
-  </si>
-  <si>
     <t>Depression</t>
   </si>
   <si>
@@ -145,6 +142,9 @@
   </si>
   <si>
     <t>Westminster, City of</t>
+  </si>
+  <si>
+    <t>Name</t>
   </si>
 </sst>
 </file>
@@ -533,9 +533,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CE2C7CF1-A88E-274C-B728-638B4149C5AD}">
   <dimension ref="A1:D35"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A35" sqref="A35"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
@@ -547,21 +545,21 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>1</v>
+        <v>36</v>
       </c>
       <c r="B1" t="s">
         <v>0</v>
       </c>
       <c r="C1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" t="s">
         <v>2</v>
-      </c>
-      <c r="D1" t="s">
-        <v>3</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B2" s="1">
         <v>2</v>
@@ -575,7 +573,7 @@
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B3" s="1">
         <v>13</v>
@@ -589,7 +587,7 @@
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B4" s="1">
         <v>32</v>
@@ -603,7 +601,7 @@
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B5" s="1">
         <v>14</v>
@@ -617,7 +615,7 @@
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B6" s="1">
         <v>25</v>
@@ -631,7 +629,7 @@
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B7" s="1">
         <v>28</v>
@@ -645,7 +643,7 @@
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B8" s="1">
         <v>23</v>
@@ -659,7 +657,7 @@
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B9" s="1">
         <v>36</v>
@@ -673,7 +671,7 @@
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B10" s="1">
         <v>12</v>
@@ -687,7 +685,7 @@
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B11" s="1">
         <v>13</v>
@@ -701,7 +699,7 @@
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B12" s="1">
         <v>14</v>
@@ -715,7 +713,7 @@
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B13" s="1">
         <v>10</v>
@@ -729,7 +727,7 @@
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B14" s="1">
         <v>9</v>
@@ -743,7 +741,7 @@
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B15" s="1">
         <v>31</v>
@@ -757,7 +755,7 @@
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B16" s="1">
         <v>13</v>
@@ -771,7 +769,7 @@
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B17" s="1">
         <v>19</v>
@@ -785,7 +783,7 @@
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B18" s="1">
         <v>8</v>
@@ -799,7 +797,7 @@
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B19" s="1">
         <v>6</v>
@@ -813,7 +811,7 @@
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B20" s="1">
         <v>16</v>
@@ -827,7 +825,7 @@
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B21" s="1">
         <v>12</v>
@@ -841,7 +839,7 @@
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B22" s="1">
         <v>4</v>
@@ -855,7 +853,7 @@
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B23" s="1">
         <v>19</v>
@@ -869,7 +867,7 @@
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B24" s="1">
         <v>15</v>
@@ -883,7 +881,7 @@
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B25" s="1">
         <v>11</v>
@@ -897,7 +895,7 @@
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B26" s="1">
         <v>23</v>
@@ -911,7 +909,7 @@
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B27" s="1">
         <v>15</v>
@@ -925,7 +923,7 @@
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B28" s="1">
         <v>6</v>
@@ -939,7 +937,7 @@
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B29" s="1">
         <v>31</v>
@@ -953,7 +951,7 @@
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B30" s="1">
         <v>11</v>
@@ -967,7 +965,7 @@
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B31" s="1">
         <v>22</v>
@@ -981,7 +979,7 @@
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B32" s="1">
         <v>20</v>
@@ -995,7 +993,7 @@
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B33" s="1">
         <v>21</v>
@@ -1009,7 +1007,7 @@
     </row>
     <row r="34" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B34" s="1">
         <v>17</v>

</xml_diff>